<commit_message>
Time table generator code added
</commit_message>
<xml_diff>
--- a/AI - Timetable.xlsx
+++ b/AI - Timetable.xlsx
@@ -5,33 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\AI-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Prerna Tulsiani\COEP\Sem5\AI\Final_Project\AI-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F26855-1653-4833-BB6D-5F1E803482AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DDA64A-7E77-4C03-B0A8-CFA0633345F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Faculty" sheetId="1" r:id="rId1"/>
     <sheet name="Courses" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="218">
   <si>
     <t>Sr. no</t>
   </si>
@@ -632,6 +622,60 @@
   </si>
   <si>
     <t>CSE_117</t>
+  </si>
+  <si>
+    <t>Course_short_name</t>
+  </si>
+  <si>
+    <t>PSE</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>SEMP - 1</t>
+  </si>
+  <si>
+    <t>SEMP TUT - 1</t>
+  </si>
+  <si>
+    <t>DBMS</t>
+  </si>
+  <si>
+    <t>DBMS LAB</t>
+  </si>
+  <si>
+    <t>AI LAB</t>
+  </si>
+  <si>
+    <t>CN LAB</t>
+  </si>
+  <si>
+    <t>OS LAB</t>
+  </si>
+  <si>
+    <t>DS LAB</t>
+  </si>
+  <si>
+    <t>SE - 2</t>
+  </si>
+  <si>
+    <t>DE - 1</t>
+  </si>
+  <si>
+    <t>DE - 1 LAB</t>
   </si>
 </sst>
 </file>
@@ -683,7 +727,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -706,11 +750,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -721,6 +776,9 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1484,18 +1542,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="E2" sqref="E2:E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="46.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1514,8 +1573,11 @@
       <c r="F1" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1529,13 +1591,16 @@
         <v>5</v>
       </c>
       <c r="E2" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F2" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1549,13 +1614,16 @@
         <v>5</v>
       </c>
       <c r="E3" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1569,13 +1637,16 @@
         <v>5</v>
       </c>
       <c r="E4" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -1589,13 +1660,16 @@
         <v>5</v>
       </c>
       <c r="E5" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F5" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -1609,13 +1683,16 @@
         <v>5</v>
       </c>
       <c r="E6" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F6" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -1629,13 +1706,16 @@
         <v>5</v>
       </c>
       <c r="E7" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1649,13 +1729,16 @@
         <v>5</v>
       </c>
       <c r="E8" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F8" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -1669,13 +1752,16 @@
         <v>5</v>
       </c>
       <c r="E9" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -1689,13 +1775,16 @@
         <v>5</v>
       </c>
       <c r="E10" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F10" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -1709,13 +1798,16 @@
         <v>5</v>
       </c>
       <c r="E11" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -1729,13 +1821,16 @@
         <v>6</v>
       </c>
       <c r="E12" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F12" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
@@ -1749,13 +1844,16 @@
         <v>6</v>
       </c>
       <c r="E13" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G13" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
@@ -1769,13 +1867,16 @@
         <v>6</v>
       </c>
       <c r="E14" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F14" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
@@ -1789,13 +1890,16 @@
         <v>6</v>
       </c>
       <c r="E15" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G15" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
@@ -1809,13 +1913,16 @@
         <v>6</v>
       </c>
       <c r="E16" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
@@ -1829,13 +1936,16 @@
         <v>6</v>
       </c>
       <c r="E17" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F17" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>91</v>
       </c>
@@ -1849,13 +1959,16 @@
         <v>6</v>
       </c>
       <c r="E18" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G18" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
@@ -1875,7 +1988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>24</v>
       </c>
@@ -1895,7 +2008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
@@ -1915,7 +2028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
@@ -1935,7 +2048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
@@ -1955,7 +2068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>32</v>
       </c>
@@ -1975,7 +2088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>34</v>
       </c>
@@ -1995,7 +2108,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
@@ -2015,7 +2128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>38</v>
       </c>
@@ -2035,7 +2148,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>21</v>
       </c>
@@ -2055,7 +2168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>24</v>
       </c>
@@ -2075,7 +2188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>26</v>
       </c>
@@ -2095,7 +2208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>28</v>
       </c>
@@ -2115,7 +2228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>30</v>
       </c>
@@ -2589,7 +2702,7 @@
         <v>5</v>
       </c>
       <c r="E55" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F55" s="4">
         <v>3</v>
@@ -2609,7 +2722,7 @@
         <v>5</v>
       </c>
       <c r="E56" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F56" s="4">
         <v>3</v>
@@ -2629,7 +2742,7 @@
         <v>5</v>
       </c>
       <c r="E57" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F57" s="4">
         <v>3</v>
@@ -2649,7 +2762,7 @@
         <v>5</v>
       </c>
       <c r="E58" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F58" s="4">
         <v>3</v>
@@ -2669,7 +2782,7 @@
         <v>5</v>
       </c>
       <c r="E59" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F59" s="4">
         <v>3</v>
@@ -2689,7 +2802,7 @@
         <v>5</v>
       </c>
       <c r="E60" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F60" s="4">
         <v>3</v>
@@ -2709,7 +2822,7 @@
         <v>5</v>
       </c>
       <c r="E61" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F61" s="4">
         <v>3</v>
@@ -2729,7 +2842,7 @@
         <v>5</v>
       </c>
       <c r="E62" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F62" s="4">
         <v>3</v>
@@ -2749,7 +2862,7 @@
         <v>5</v>
       </c>
       <c r="E63" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" s="4">
         <v>1</v>
@@ -2769,7 +2882,7 @@
         <v>5</v>
       </c>
       <c r="E64" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" s="4">
         <v>1</v>
@@ -2789,7 +2902,7 @@
         <v>5</v>
       </c>
       <c r="E65" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" s="4">
         <v>1</v>
@@ -2809,7 +2922,7 @@
         <v>5</v>
       </c>
       <c r="E66" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" s="4">
         <v>1</v>
@@ -2829,7 +2942,7 @@
         <v>5</v>
       </c>
       <c r="E67" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" s="4">
         <v>1</v>
@@ -2849,7 +2962,7 @@
         <v>5</v>
       </c>
       <c r="E68" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" s="4">
         <v>1</v>
@@ -2869,7 +2982,7 @@
         <v>5</v>
       </c>
       <c r="E69" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" s="4">
         <v>1</v>
@@ -2889,7 +3002,7 @@
         <v>5</v>
       </c>
       <c r="E70" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" s="4">
         <v>1</v>
@@ -2909,7 +3022,7 @@
         <v>6</v>
       </c>
       <c r="E71" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F71" s="4">
         <v>3</v>
@@ -2929,7 +3042,7 @@
         <v>6</v>
       </c>
       <c r="E72" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F72" s="4">
         <v>3</v>
@@ -2949,7 +3062,7 @@
         <v>6</v>
       </c>
       <c r="E73" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F73" s="4">
         <v>3</v>
@@ -2969,7 +3082,7 @@
         <v>6</v>
       </c>
       <c r="E74" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F74" s="4">
         <v>3</v>
@@ -2989,7 +3102,7 @@
         <v>6</v>
       </c>
       <c r="E75" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" s="4">
         <v>1</v>
@@ -3009,7 +3122,7 @@
         <v>6</v>
       </c>
       <c r="E76" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" s="4">
         <v>1</v>
@@ -3029,7 +3142,7 @@
         <v>6</v>
       </c>
       <c r="E77" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" s="4">
         <v>1</v>

</xml_diff>

<commit_message>
Teacher availability constraint added
</commit_message>
<xml_diff>
--- a/AI - Timetable.xlsx
+++ b/AI - Timetable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\AI-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8123EAE0-8224-4627-9151-23040C4A8C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD21BDD-A2B9-4931-AE01-18D8721E273F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="301">
   <si>
     <t>Sr. no</t>
   </si>
@@ -352,9 +352,6 @@
     <t>Software Engineering 2</t>
   </si>
   <si>
-    <t>SE - 2</t>
-  </si>
-  <si>
     <t>CSE_116</t>
   </si>
   <si>
@@ -376,10 +373,6 @@
     <t>ENTC_101</t>
   </si>
   <si>
-    <t>R and Python Programming
-Lab</t>
-  </si>
-  <si>
     <t>ENTC_102</t>
   </si>
   <si>
@@ -686,9 +679,6 @@
     <t>SEMP LAB - 1</t>
   </si>
   <si>
-    <t>R &amp; Python Lab</t>
-  </si>
-  <si>
     <t>Dig. Analytics</t>
   </si>
   <si>
@@ -827,9 +817,6 @@
     <t>ETnEC Lab</t>
   </si>
   <si>
-    <t>IF</t>
-  </si>
-  <si>
     <t>Conf and Processor</t>
   </si>
   <si>
@@ -885,13 +872,70 @@
   </si>
   <si>
     <t>Mini Proj</t>
+  </si>
+  <si>
+    <t>R and Python Programming</t>
+  </si>
+  <si>
+    <t>R &amp; Python</t>
+  </si>
+  <si>
+    <t>SE - 2 LAB</t>
+  </si>
+  <si>
+    <t>CSE_118</t>
+  </si>
+  <si>
+    <t>CSE_119</t>
+  </si>
+  <si>
+    <t>CSE_120</t>
+  </si>
+  <si>
+    <t>CSE_121</t>
+  </si>
+  <si>
+    <t>Design and Analysis of Algorithms Laboratory</t>
+  </si>
+  <si>
+    <t>DAA LAB</t>
+  </si>
+  <si>
+    <t>Design and Analysis of Algorithms</t>
+  </si>
+  <si>
+    <t>DAA</t>
+  </si>
+  <si>
+    <t>Introduction to Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>IAI</t>
+  </si>
+  <si>
+    <t>Cyber Security</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>ENTC_141</t>
+  </si>
+  <si>
+    <t>VLSI LAB</t>
+  </si>
+  <si>
+    <t>VLSI Laboratory</t>
+  </si>
+  <si>
+    <t>IF Lab</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -903,6 +947,11 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1334,7 +1383,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1376,7 +1425,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="1">
-        <v>0.41666666666666669</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="F2" s="1">
         <v>0.75</v>
@@ -1396,10 +1445,10 @@
         <v>8</v>
       </c>
       <c r="E3" s="1">
-        <v>0.41666666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="F3" s="1">
-        <v>0.75</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -1416,7 +1465,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="1">
-        <v>0.41666666666666669</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="F4" s="1">
         <v>0.75</v>
@@ -1439,7 +1488,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="F5" s="1">
-        <v>0.75</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -1456,10 +1505,10 @@
         <v>8</v>
       </c>
       <c r="E6" s="1">
-        <v>0.41666666666666669</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="F6" s="1">
-        <v>0.75</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -1516,10 +1565,10 @@
         <v>8</v>
       </c>
       <c r="E9" s="1">
-        <v>0.41666666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="F9" s="1">
-        <v>0.75</v>
+        <v>0.70833333333333337</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -1539,7 +1588,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="F10" s="1">
-        <v>0.75</v>
+        <v>0.70833333333333337</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -1556,10 +1605,10 @@
         <v>25</v>
       </c>
       <c r="E11" s="1">
-        <v>0.41666666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="F11" s="1">
-        <v>0.75</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -1576,7 +1625,7 @@
         <v>25</v>
       </c>
       <c r="E12" s="1">
-        <v>0.41666666666666669</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="F12" s="1">
         <v>0.75</v>
@@ -1599,7 +1648,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="F13" s="1">
-        <v>0.75</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -1619,7 +1668,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="F14" s="1">
-        <v>0.75</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -1676,10 +1725,10 @@
         <v>25</v>
       </c>
       <c r="E17" s="1">
-        <v>0.41666666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="F17" s="1">
-        <v>0.75</v>
+        <v>0.70833333333333337</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -1736,10 +1785,10 @@
         <v>44</v>
       </c>
       <c r="E20" s="1">
-        <v>0.41666666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="F20" s="1">
-        <v>0.75</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -1756,7 +1805,7 @@
         <v>44</v>
       </c>
       <c r="E21" s="1">
-        <v>0.41666666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="F21" s="1">
         <v>0.75</v>
@@ -1779,7 +1828,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="F22" s="1">
-        <v>0.75</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -1799,7 +1848,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="F23" s="1">
-        <v>0.75</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -1819,7 +1868,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="F24" s="1">
-        <v>0.75</v>
+        <v>0.70833333333333337</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -1836,7 +1885,7 @@
         <v>44</v>
       </c>
       <c r="E25" s="1">
-        <v>0.41666666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="F25" s="1">
         <v>0.75</v>
@@ -1856,10 +1905,10 @@
         <v>44</v>
       </c>
       <c r="E26" s="1">
-        <v>0.41666666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="F26" s="1">
-        <v>0.75</v>
+        <v>0.70833333333333337</v>
       </c>
     </row>
   </sheetData>
@@ -1870,10 +1919,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G77"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I73" sqref="I73"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1948,7 +1997,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -2247,7 +2296,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>108</v>
+        <v>284</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -2255,10 +2304,10 @@
         <v>19</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="D17" s="3">
         <v>6</v>
@@ -2270,18 +2319,18 @@
         <v>3</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>113</v>
+        <v>289</v>
       </c>
       <c r="D18" s="3">
         <v>6</v>
@@ -2293,67 +2342,67 @@
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>115</v>
+        <v>285</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>116</v>
+        <v>291</v>
       </c>
       <c r="D19" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E19" s="3">
         <v>1</v>
       </c>
       <c r="F19" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>219</v>
+        <v>292</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>117</v>
+        <v>286</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>118</v>
+        <v>293</v>
       </c>
       <c r="D20" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E20" s="3">
         <v>1</v>
       </c>
       <c r="F20" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>220</v>
+        <v>294</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>119</v>
+        <v>287</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>120</v>
+        <v>295</v>
       </c>
       <c r="D21" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E21" s="3">
         <v>1</v>
@@ -2362,41 +2411,41 @@
         <v>3</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>221</v>
+        <v>296</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>121</v>
+        <v>288</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D22" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E22" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F22" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>222</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>124</v>
+        <v>282</v>
       </c>
       <c r="D23" s="3">
         <v>5</v>
@@ -2405,21 +2454,21 @@
         <v>1</v>
       </c>
       <c r="F23" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>267</v>
+        <v>283</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="D24" s="3">
         <v>5</v>
@@ -2428,113 +2477,113 @@
         <v>1</v>
       </c>
       <c r="F24" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>268</v>
+        <v>217</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="D25" s="3">
         <v>5</v>
       </c>
       <c r="E25" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D26" s="3">
         <v>5</v>
       </c>
       <c r="E26" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="D27" s="3">
         <v>5</v>
       </c>
       <c r="E27" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>225</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>269</v>
+        <v>124</v>
       </c>
       <c r="D28" s="3">
         <v>5</v>
       </c>
       <c r="E28" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>271</v>
+        <v>126</v>
       </c>
       <c r="D29" s="3">
         <v>5</v>
@@ -2546,110 +2595,110 @@
         <v>1</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>272</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D30" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E30" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F30" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D31" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E31" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F31" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>138</v>
+        <v>265</v>
       </c>
       <c r="D32" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E32" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F32" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>227</v>
+        <v>266</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>140</v>
+        <v>267</v>
       </c>
       <c r="D33" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E33" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F33" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>228</v>
+        <v>268</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D34" s="3">
         <v>6</v>
@@ -2661,18 +2710,18 @@
         <v>3</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="D35" s="3">
         <v>6</v>
@@ -2681,21 +2730,21 @@
         <v>1</v>
       </c>
       <c r="F35" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="D36" s="3">
         <v>6</v>
@@ -2707,53 +2756,53 @@
         <v>3</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="D37" s="3">
         <v>6</v>
       </c>
       <c r="E37" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D38" s="3">
         <v>6</v>
       </c>
       <c r="E38" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -2761,59 +2810,59 @@
         <v>34</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>275</v>
+        <v>142</v>
       </c>
       <c r="D39" s="3">
         <v>6</v>
       </c>
       <c r="E39" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>276</v>
+        <v>227</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>277</v>
+        <v>109</v>
       </c>
       <c r="D40" s="3">
         <v>6</v>
       </c>
       <c r="E40" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>278</v>
+        <v>228</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>151</v>
+        <v>299</v>
       </c>
       <c r="D41" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E41" s="3">
         <v>2</v>
@@ -2822,76 +2871,76 @@
         <v>1</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>234</v>
+        <v>298</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D42" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E42" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F42" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D43" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E43" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F43" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>157</v>
+        <v>271</v>
       </c>
       <c r="D44" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E44" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F44" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>237</v>
+        <v>272</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -2899,128 +2948,128 @@
         <v>32</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>159</v>
+        <v>273</v>
       </c>
       <c r="D45" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E45" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F45" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>238</v>
+        <v>274</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="D46" s="3">
         <v>4</v>
       </c>
       <c r="E46" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F46" s="3">
         <v>1</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="D47" s="3">
         <v>4</v>
       </c>
       <c r="E47" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="D48" s="3">
         <v>4</v>
       </c>
       <c r="E48" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="D49" s="3">
         <v>4</v>
       </c>
       <c r="E49" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="D50" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E50" s="3">
         <v>1</v>
@@ -3029,110 +3078,110 @@
         <v>3</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="D51" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E51" s="3">
         <v>1</v>
       </c>
       <c r="F51" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D52" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E52" s="3">
         <v>2</v>
       </c>
       <c r="F52" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="D53" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E53" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F53" s="3">
         <v>1</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="D54" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E54" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F54" s="3">
         <v>1</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>273</v>
+        <v>176</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="D55" s="3">
         <v>3</v>
@@ -3141,44 +3190,44 @@
         <v>1</v>
       </c>
       <c r="F55" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>274</v>
+        <v>178</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="D56" s="3">
         <v>3</v>
       </c>
       <c r="E56" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>279</v>
+        <v>180</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="D57" s="3">
         <v>3</v>
@@ -3187,148 +3236,148 @@
         <v>2</v>
       </c>
       <c r="F57" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>280</v>
+        <v>182</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="D58" s="3">
         <v>3</v>
       </c>
       <c r="E58" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F58" s="3">
         <v>1</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>186</v>
+        <v>269</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="D59" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E59" s="3">
         <v>1</v>
       </c>
       <c r="F59" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>188</v>
+        <v>270</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="D60" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E60" s="3">
         <v>1</v>
       </c>
       <c r="F60" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>190</v>
+        <v>275</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="D61" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E61" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F61" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>192</v>
+        <v>276</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="D62" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E62" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F62" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>194</v>
+        <v>297</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="D63" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E63" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F63" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -3336,22 +3385,22 @@
         <v>42</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="D64" s="3">
         <v>5</v>
       </c>
       <c r="E64" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F64" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -3359,68 +3408,68 @@
         <v>45</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="D65" s="3">
         <v>5</v>
       </c>
       <c r="E65" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="D66" s="3">
         <v>5</v>
       </c>
       <c r="E66" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="D67" s="3">
         <v>5</v>
       </c>
       <c r="E67" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -3428,22 +3477,22 @@
         <v>57</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="D68" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E68" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -3451,22 +3500,22 @@
         <v>42</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="D69" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E69" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F69" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -3474,22 +3523,22 @@
         <v>45</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="D70" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E70" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F70" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -3497,22 +3546,22 @@
         <v>47</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="D71" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E71" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F71" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -3520,33 +3569,33 @@
         <v>49</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="D72" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E72" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F72" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="D73" s="3">
         <v>6</v>
@@ -3558,102 +3607,204 @@
         <v>1</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="D74" s="3">
         <v>6</v>
       </c>
       <c r="E74" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>281</v>
+        <v>205</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>282</v>
+        <v>206</v>
       </c>
       <c r="D75" s="3">
         <v>6</v>
       </c>
       <c r="E75" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>283</v>
+        <v>259</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>284</v>
+        <v>207</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="D76" s="3">
         <v>6</v>
       </c>
       <c r="E76" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>285</v>
+        <v>260</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>284</v>
+        <v>209</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="D77" s="3">
         <v>6</v>
       </c>
       <c r="E77" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>285</v>
-      </c>
+        <v>261</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D78" s="3">
+        <v>6</v>
+      </c>
+      <c r="E78" s="3">
+        <v>2</v>
+      </c>
+      <c r="F78" s="3">
+        <v>1</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D79" s="3">
+        <v>6</v>
+      </c>
+      <c r="E79" s="3">
+        <v>2</v>
+      </c>
+      <c r="F79" s="3">
+        <v>1</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D80" s="3">
+        <v>6</v>
+      </c>
+      <c r="E80" s="3">
+        <v>2</v>
+      </c>
+      <c r="F80" s="3">
+        <v>1</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D81" s="3">
+        <v>6</v>
+      </c>
+      <c r="E81" s="3">
+        <v>2</v>
+      </c>
+      <c r="F81" s="3">
+        <v>1</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="2"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>